<commit_message>
updates trap data and metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/tisdale_trap_metadata.xlsx
+++ b/data-raw/metadata/tisdale_trap_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-tisdale-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57992CA7-7A54-40B0-A54B-118FABA7D26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F663DD9-831B-42E8-A351-A5BD201466C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="68">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -225,11 +225,20 @@
   <si>
     <t>2022-09-04 10:00:57</t>
   </si>
+  <si>
+    <t>visitTime2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date and time of day associated with the end of trap visit. Definition varies based on visitType. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -296,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -340,6 +349,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -830,28 +840,34 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="21">
+        <v>40366.542060185187</v>
+      </c>
+      <c r="M7" s="21">
+        <v>45540.417326331015</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -866,116 +882,106 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="3">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3">
-        <v>28393</v>
-      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -992,10 +998,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1010,7 +1016,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>35</v>
@@ -1022,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3">
-        <v>20.5</v>
+        <v>3195559</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1040,7 +1046,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
@@ -1070,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>195</v>
+        <v>20.5</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1088,28 +1094,38 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>195</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1126,38 +1142,28 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3">
-        <v>1</v>
-      </c>
-      <c r="M14" s="3">
-        <v>1</v>
-      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1174,10 +1180,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1192,7 +1198,7 @@
         <v>32</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>35</v>
@@ -1201,10 +1207,10 @@
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
       <c r="L15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="3">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1222,10 +1228,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1240,7 +1246,7 @@
         <v>32</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>35</v>
@@ -1249,10 +1255,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
       <c r="L16" s="3">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="M16" s="3">
-        <v>551</v>
+        <v>63</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1268,12 +1274,12 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
-        <v>46</v>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>44</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>47</v>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1287,8 +1293,8 @@
       <c r="F17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>48</v>
+      <c r="G17" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>35</v>
@@ -1297,52 +1303,72 @@
       <c r="J17" s="3"/>
       <c r="K17" s="2"/>
       <c r="L17" s="3">
-        <v>0.97</v>
+        <v>1.7</v>
       </c>
       <c r="M17" s="3">
-        <v>2079</v>
+        <v>551</v>
       </c>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I18" s="2"/>
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
+      <c r="L18" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="M18" s="3">
+        <v>2079</v>
+      </c>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
@@ -1877,7 +1903,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="19"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1905,7 +1931,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="20"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1933,7 +1959,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="19"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -1961,7 +1987,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="20"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -1989,7 +2015,7 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="4"/>
+      <c r="A42" s="20"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
@@ -2941,7 +2967,7 @@
       <c r="Z75" s="1"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="1"/>
+      <c r="A76" s="4"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="2"/>
@@ -28868,22 +28894,50 @@
       <c r="Y1001" s="1"/>
       <c r="Z1001" s="1"/>
     </row>
+    <row r="1002" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="2"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="3"/>
+      <c r="G1002" s="3"/>
+      <c r="H1002" s="3"/>
+      <c r="I1002" s="2"/>
+      <c r="J1002" s="3"/>
+      <c r="K1002" s="2"/>
+      <c r="L1002" s="3"/>
+      <c r="M1002" s="3"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E1001" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E1002" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F1001" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F1002" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C1:C46" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C59:C1002 C1:C47" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H1001" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H1002" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
transforms watertemp to single unit, updates trap metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/tisdale_trap_metadata.xlsx
+++ b/data-raw/metadata/tisdale_trap_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-tisdale-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2533A63-94F4-412F-9431-F68D941482A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27605432-B9E6-4585-99B0-D88EEDF2CAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22005" yWindow="3150" windowWidth="18600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="1880" windowWidth="19200" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="83">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -169,12 +169,6 @@
     <t>turbidity</t>
   </si>
   <si>
-    <t>Turbidity measured at trap</t>
-  </si>
-  <si>
-    <t>NTU</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -211,9 +205,6 @@
     <t>Code for description of how well trap is functioning when visit to trap began. Levels = c("Trap functioning normally", "Trap stopped functioning", "Trap functioning, but not normally", "Trap not in service", "Not recorded")</t>
   </si>
   <si>
-    <t>fahrenheit</t>
-  </si>
-  <si>
     <t>Foreign key to the CAMP ProjectDescription table.  All data associated with this package will have a ProjectDescriptionID = 10.</t>
   </si>
   <si>
@@ -242,6 +233,48 @@
   </si>
   <si>
     <t>2024-09-04 10:00:57</t>
+  </si>
+  <si>
+    <t>counterAtStart</t>
+  </si>
+  <si>
+    <t>Reading on the rotation counter at the start of the trap visit</t>
+  </si>
+  <si>
+    <t>celsius</t>
+  </si>
+  <si>
+    <t>lightPenetration</t>
+  </si>
+  <si>
+    <t>dissolvedOxygen</t>
+  </si>
+  <si>
+    <t>conductivity</t>
+  </si>
+  <si>
+    <t>Instantaneous light penetration measured</t>
+  </si>
+  <si>
+    <t>centimeter</t>
+  </si>
+  <si>
+    <t>Instantaneous turbidity measurement</t>
+  </si>
+  <si>
+    <t>Nephelometric Turbidity Units (NTU)</t>
+  </si>
+  <si>
+    <t>Instantaneous dissolved oxygen measurement</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Instantaneous conductivity measurement</t>
+  </si>
+  <si>
+    <t>microSiemens per centimeter</t>
   </si>
 </sst>
 </file>
@@ -317,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -360,14 +393,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -665,7 +702,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -741,7 +778,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -779,7 +816,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
@@ -837,10 +874,10 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -858,10 +895,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
@@ -905,7 +942,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -943,7 +980,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
@@ -981,7 +1018,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -1016,10 +1053,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1046,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3">
-        <v>3195559</v>
+        <v>3504561</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1064,10 +1101,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1082,7 +1119,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>35</v>
@@ -1094,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>20.5</v>
+        <v>28393</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1112,7 +1149,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>37</v>
@@ -1142,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="3">
-        <v>195</v>
+        <v>20.5</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1160,28 +1197,38 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>195</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1198,38 +1245,28 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="3">
-        <v>1</v>
-      </c>
-      <c r="M15" s="3">
-        <v>1</v>
-      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1246,10 +1283,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1264,7 +1301,7 @@
         <v>32</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>35</v>
@@ -1273,10 +1310,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
       <c r="L16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="3">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1294,10 +1331,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1312,7 +1349,7 @@
         <v>32</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>35</v>
@@ -1321,10 +1358,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="2"/>
       <c r="L17" s="3">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="M17" s="3">
-        <v>551</v>
+        <v>63</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1340,12 +1377,12 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>46</v>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>44</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>47</v>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1359,8 +1396,8 @@
       <c r="F18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>48</v>
+      <c r="G18" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>35</v>
@@ -1369,54 +1406,58 @@
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
       <c r="L18" s="3">
-        <v>0.97</v>
+        <v>1.7</v>
       </c>
       <c r="M18" s="3">
-        <v>2079</v>
+        <v>24.44</v>
       </c>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>67</v>
+      <c r="A19" s="25" t="s">
+        <v>72</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>68</v>
+      <c r="B19" s="25" t="s">
+        <v>75</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>25</v>
+      <c r="C19" s="25" t="s">
+        <v>32</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>25</v>
+      <c r="E19" s="25" t="s">
+        <v>33</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6" t="s">
-        <v>26</v>
+      <c r="F19" s="24" t="s">
+        <v>32</v>
       </c>
+      <c r="G19" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="23">
-        <v>40365.542060185187</v>
+      <c r="L19" s="3">
+        <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M19" s="23">
-        <v>45539.417326388888</v>
+      <c r="M19" s="3">
+        <v>32.4</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1432,120 +1473,180 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
-        <v>69</v>
+    <row r="20" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="27" t="s">
+        <v>46</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>70</v>
+      <c r="B20" s="25" t="s">
+        <v>77</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>25</v>
+      <c r="C20" s="25" t="s">
+        <v>32</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>25</v>
+      <c r="E20" s="25" t="s">
+        <v>33</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="6" t="s">
-        <v>26</v>
+      <c r="F20" s="24" t="s">
+        <v>32</v>
       </c>
+      <c r="G20" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="23">
-        <v>40365.542060185187</v>
+      <c r="L20" s="3">
+        <v>0.97</v>
       </c>
-      <c r="M20" s="23">
-        <v>45539.417326388888</v>
+      <c r="M20" s="3">
+        <v>2079</v>
       </c>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="L21" s="3">
+        <v>1</v>
+      </c>
+      <c r="M21" s="3">
+        <v>1</v>
+      </c>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+    </row>
+    <row r="22" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I22" s="2"/>
       <c r="J22" s="3"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="L22" s="3">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3">
+        <v>1</v>
+      </c>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
+      <c r="A23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="L23" s="21">
+        <v>40365.542060185187</v>
+      </c>
+      <c r="M23" s="21">
+        <v>45539.417326388888</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1561,19 +1662,35 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
+      <c r="A24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="L24" s="21">
+        <v>40365.542060185187</v>
+      </c>
+      <c r="M24" s="21">
+        <v>45539.417326388888</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1981,7 +2098,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="20"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -2009,7 +2126,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="21"/>
+      <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -2037,7 +2154,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="20"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -2065,7 +2182,7 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="21"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
@@ -2093,7 +2210,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="4"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
@@ -2121,7 +2238,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="4"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
@@ -2149,7 +2266,7 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="4"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
@@ -2177,7 +2294,7 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
@@ -3045,7 +3162,7 @@
       <c r="Z76" s="1"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="1"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="2"/>
@@ -3073,7 +3190,7 @@
       <c r="Z77" s="1"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="1"/>
+      <c r="A78" s="4"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="2"/>
@@ -3101,7 +3218,7 @@
       <c r="Z78" s="1"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="1"/>
+      <c r="A79" s="4"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="2"/>
@@ -3129,7 +3246,7 @@
       <c r="Z79" s="1"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
+      <c r="A80" s="4"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="2"/>
@@ -28972,22 +29089,134 @@
       <c r="Y1002" s="1"/>
       <c r="Z1002" s="1"/>
     </row>
+    <row r="1003" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="3"/>
+      <c r="G1003" s="3"/>
+      <c r="H1003" s="3"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="3"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="3"/>
+      <c r="M1003" s="3"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+      <c r="S1003" s="1"/>
+      <c r="T1003" s="1"/>
+      <c r="U1003" s="1"/>
+      <c r="V1003" s="1"/>
+      <c r="W1003" s="1"/>
+      <c r="X1003" s="1"/>
+      <c r="Y1003" s="1"/>
+      <c r="Z1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="3"/>
+      <c r="G1004" s="3"/>
+      <c r="H1004" s="3"/>
+      <c r="I1004" s="2"/>
+      <c r="J1004" s="3"/>
+      <c r="K1004" s="2"/>
+      <c r="L1004" s="3"/>
+      <c r="M1004" s="3"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+      <c r="S1004" s="1"/>
+      <c r="T1004" s="1"/>
+      <c r="U1004" s="1"/>
+      <c r="V1004" s="1"/>
+      <c r="W1004" s="1"/>
+      <c r="X1004" s="1"/>
+      <c r="Y1004" s="1"/>
+      <c r="Z1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="2"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="3"/>
+      <c r="G1005" s="3"/>
+      <c r="H1005" s="3"/>
+      <c r="I1005" s="2"/>
+      <c r="J1005" s="3"/>
+      <c r="K1005" s="2"/>
+      <c r="L1005" s="3"/>
+      <c r="M1005" s="3"/>
+      <c r="N1005" s="1"/>
+      <c r="O1005" s="1"/>
+      <c r="P1005" s="1"/>
+      <c r="Q1005" s="1"/>
+      <c r="R1005" s="1"/>
+      <c r="S1005" s="1"/>
+      <c r="T1005" s="1"/>
+      <c r="U1005" s="1"/>
+      <c r="V1005" s="1"/>
+      <c r="W1005" s="1"/>
+      <c r="X1005" s="1"/>
+      <c r="Y1005" s="1"/>
+      <c r="Z1005" s="1"/>
+    </row>
+    <row r="1006" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="3"/>
+      <c r="G1006" s="3"/>
+      <c r="H1006" s="3"/>
+      <c r="I1006" s="2"/>
+      <c r="J1006" s="3"/>
+      <c r="K1006" s="2"/>
+      <c r="L1006" s="3"/>
+      <c r="M1006" s="3"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+      <c r="S1006" s="1"/>
+      <c r="T1006" s="1"/>
+      <c r="U1006" s="1"/>
+      <c r="V1006" s="1"/>
+      <c r="W1006" s="1"/>
+      <c r="X1006" s="1"/>
+      <c r="Y1006" s="1"/>
+      <c r="Z1006" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E1002" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E1006" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F1002" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F1006" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C59:C1002 C1:C47" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C1:C51" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H1002" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H1006" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -29014,13 +29243,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -29051,7 +29280,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>13</v>

</xml_diff>